<commit_message>
Loads of changes, especially differentiation but many things for the presentation as well
</commit_message>
<xml_diff>
--- a/STRUCTURE Results MLGs.xlsx
+++ b/STRUCTURE Results MLGs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wslch365-my.sharepoint.com/personal/lia_baumann_wsl_ch/Documents/R/truffles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A264E7C-692B-4BC3-AE2E-DF789D40B6F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{7A264E7C-692B-4BC3-AE2E-DF789D40B6F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CEBDBE60-52C4-4164-B1FE-46C873447888}"/>
   <bookViews>
-    <workbookView xWindow="43080" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{4AF5B5B8-752F-4F4A-8D00-808F0CD9F65A}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{4AF5B5B8-752F-4F4A-8D00-808F0CD9F65A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -3202,8 +3202,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2823BC7-8315-41C7-A7D8-CFE8D37D5227}">
   <dimension ref="A1:C468"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A111" workbookViewId="0">
+      <selection activeCell="C137" sqref="C137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -4731,7 +4731,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A139" s="1" t="s">
-        <v>2</v>
+        <v>23</v>
       </c>
       <c r="B139" t="s">
         <v>652</v>

</xml_diff>